<commit_message>
Make drawing and blip IDs consistent
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/ImageHandling/ImageHandling.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/ImageHandling/ImageHandling.xlsx
@@ -7,7 +7,7 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Images" sheetId="2" r:id="rId2"/>
-    <x:sheet name="MoreImages" sheetId="5" r:id="rId5"/>
+    <x:sheet name="MoreImages" sheetId="3" r:id="rId3"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -89,7 +89,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="Rf5f91c830a3946f9" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="Image10" cstate="print"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -120,7 +120,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="Re8ef5c0cc47b41f6" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="Image11" cstate="print"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -161,7 +161,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="R508c4e1acc484d2c" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="Image20" cstate="print"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -477,7 +477,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rc454d8d9336b4825"/>
+  <x:drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Image10"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
@@ -497,7 +497,7 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5e82497dc9334352"/>
+  <x:drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Image20"/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
</xml_diff>